<commit_message>
add columnValueMap to select PhpExcel value method
</commit_message>
<xml_diff>
--- a/tests/files/test.xlsx
+++ b/tests/files/test.xlsx
@@ -64,15 +64,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD\ HH:MM"/>
     <numFmt numFmtId="168" formatCode="HH:MM:SS"/>
-    <numFmt numFmtId="169" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0,_€_-;\-* #,##0,_€_-;_-* &quot;- &quot;_€_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="MMM\-YY"/>
+    <numFmt numFmtId="171" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -97,6 +99,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -104,12 +114,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2F0D9"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,7 +162,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,31 +187,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -212,6 +236,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFE2F0D9"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -220,17 +304,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="10.0816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.0816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -252,7 +336,16 @@
       <c r="F1" s="5" t="n">
         <v>0.000694444444444444</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="6" t="n">
+        <v>56743.6666666667</v>
+      </c>
+      <c r="H1" s="7" t="n">
+        <v>42736</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <f aca="false">B1+C1</f>
+        <v>2.01</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -273,7 +366,16 @@
       <c r="F2" s="5" t="n">
         <v>0.00138888888888889</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="6" t="n">
+        <v>56743.6666666667</v>
+      </c>
+      <c r="H2" s="7" t="n">
+        <v>42767</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <f aca="false">B2+C2</f>
+        <v>4.02</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -294,6 +396,16 @@
       <c r="F3" s="5" t="n">
         <v>0.00208333333333333</v>
       </c>
+      <c r="G3" s="6" t="n">
+        <v>46043.6666666667</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>42795</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <f aca="false">B3+C3</f>
+        <v>6.03</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -314,6 +426,16 @@
       <c r="F4" s="5" t="n">
         <v>0.00277777777777778</v>
       </c>
+      <c r="G4" s="6" t="n">
+        <v>56743.6666666667</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>42826</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <f aca="false">B4+C4</f>
+        <v>8.04</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -334,14 +456,24 @@
       <c r="F5" s="5" t="n">
         <v>0.00347222222222222</v>
       </c>
+      <c r="G5" s="6" t="n">
+        <v>47043.6666666667</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>42856</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <f aca="false">B5+C5</f>
+        <v>10.05</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regularna"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -359,31 +491,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="10.0816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.0816326530612"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -404,7 +536,7 @@
       <c r="F2" s="5" t="n">
         <v>0.000694444444444444</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -425,7 +557,7 @@
       <c r="F3" s="5" t="n">
         <v>0.00138888888888889</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -490,10 +622,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regularna"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -511,24 +643,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.82142857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="13" t="n">
+      <c r="B1" s="15" t="n">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regularna"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>